<commit_message>
DND Excel Submitted with demo graph completed Express on to EJS, React restarted.
</commit_message>
<xml_diff>
--- a/DND/FINAL EXCEL/Sub-Category-Debit-Total-Final-April.xlsx
+++ b/DND/FINAL EXCEL/Sub-Category-Debit-Total-Final-April.xlsx
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -265,6 +265,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -572,16 +573,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -718,7 +720,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="6">
-        <v>28100</v>
+        <v>27760</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>